<commit_message>
Updated Builder AV example
</commit_message>
<xml_diff>
--- a/distribution/getwrite/experiments/Builder_AV_Example/conditions/trial_conditions.xlsx
+++ b/distribution/getwrite/experiments/Builder_AV_Example/conditions/trial_conditions.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t xml:space="preserve">ROW_INDEX</t>
   </si>
@@ -48,7 +48,25 @@
     <t xml:space="preserve">DV_TRIAL_END</t>
   </si>
   <si>
-    <t xml:space="preserve">0.5</t>
+    <t xml:space="preserve">2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">go.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line768.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a2z_upper_inst.wav</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line768x3.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">drawcircles.wav</t>
@@ -57,7 +75,7 @@
     <t xml:space="preserve">CirclesCCW.mp4</t>
   </si>
   <si>
-    <t xml:space="preserve">greendot.png</t>
+    <t xml:space="preserve">green_dot.png</t>
   </si>
 </sst>
 </file>
@@ -69,7 +87,7 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -172,12 +190,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -327,7 +339,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,10 +349,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -437,10 +445,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -516,14 +524,14 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>-1.1</v>
@@ -540,16 +548,16 @@
         <v>-1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>-1.1</v>
@@ -566,21 +574,73 @@
         <v>-1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>-1.1</v>
       </c>
       <c r="H5" s="0" t="n">
+        <v>-1.1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>-1.1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>-1.1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>-1.1</v>
+      </c>
+      <c r="H7" s="0" t="n">
         <v>-1.1</v>
       </c>
     </row>

</xml_diff>